<commit_message>
Add aws_step_EC2 file with install jenkins+nginx step
</commit_message>
<xml_diff>
--- a/PDP.xlsx
+++ b/PDP.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E90EB2-7857-4D13-A26D-F0D237407716}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{F4E90EB2-7857-4D13-A26D-F0D237407716}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{CE886062-DC5F-45A6-BA48-1C77FD0EEF97}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="936" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>#</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Create instance with Jenkins server aws cli with nginx</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,7 +409,7 @@
     <col min="2" max="2" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,54 +417,64 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
+    <row r="6" spans="1:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>